<commit_message>
auto:remove some sections from the in-person visit
</commit_message>
<xml_diff>
--- a/config/forms/app/routine.xlsx
+++ b/config/forms/app/routine.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="78">
   <si>
     <t>type</t>
   </si>
@@ -143,12 +143,6 @@
 </t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>Display any open Tasks</t>
-  </si>
-  <si>
     <t>select_one yes_no</t>
   </si>
   <si>
@@ -158,17 +152,6 @@
     <t>Have you reviewed the Tasks that are due for this client?</t>
   </si>
   <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>display_dates</t>
-  </si>
-  <si>
-    <t>Display dates
-Level of Care Assessment Form:
-SRQ:</t>
-  </si>
-  <si>
     <t>select_one status</t>
   </si>
   <si>
@@ -256,7 +239,7 @@
     <t>default_language</t>
   </si>
   <si>
-    <t xml:space="preserve"> Routine Visit </t>
+    <t>Form - In-person Visit</t>
   </si>
   <si>
     <t>pages</t>
@@ -1443,14 +1426,14 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="2" t="s">
+      <c r="A24" s="11" t="s">
         <v>42</v>
       </c>
+      <c r="B24" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="C24" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1478,13 +1461,13 @@
     </row>
     <row r="25">
       <c r="A25" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1512,7 +1495,7 @@
     </row>
     <row r="26">
       <c r="A26" s="11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>48</v>
@@ -1546,13 +1529,13 @@
     </row>
     <row r="27">
       <c r="A27" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="C27" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1579,15 +1562,11 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28">
-      <c r="A28" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>54</v>
-      </c>
+      <c r="A28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1613,15 +1592,9 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>56</v>
-      </c>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -1646,64 +1619,6 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
     </row>
-    <row r="30">
-      <c r="A30" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="2"/>
-      <c r="U30" s="2"/>
-      <c r="V30" s="2"/>
-      <c r="W30" s="2"/>
-      <c r="X30" s="2"/>
-      <c r="Y30" s="2"/>
-      <c r="Z30" s="2"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
-      <c r="X31" s="2"/>
-      <c r="Y31" s="2"/>
-      <c r="Z31" s="2"/>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1721,7 +1636,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1755,68 +1670,68 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="C6" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1839,48 +1754,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="G1" s="14" t="s">
         <v>73</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>78</v>
       </c>
       <c r="H1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="16" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-11-03_09-23</v>
+        <v>2023-04-07_17-23</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H2" s="2"/>
     </row>

</xml_diff>

<commit_message>
auto:changes in the routine visit  form
</commit_message>
<xml_diff>
--- a/config/forms/app/routine.xlsx
+++ b/config/forms/app/routine.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="77">
   <si>
     <t>type</t>
   </si>
@@ -124,6 +124,27 @@
   </si>
   <si>
     <t>routine</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>in_person_date</t>
+  </si>
+  <si>
+    <t>Date of In-Person Visit</t>
+  </si>
+  <si>
+    <t>select_one status</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>What’s the client’s current clinical status?</t>
+  </si>
+  <si>
+    <t>select_one yes_no</t>
   </si>
   <si>
     <t>client</t>
@@ -133,34 +154,19 @@
 </t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>reminder</t>
   </si>
   <si>
-    <t xml:space="preserve">Have you reviewed the most recent SMS Messages with client?
+    <t xml:space="preserve">Have you reviewed the most recent SMS Messages with the client?
 </t>
   </si>
   <si>
-    <t>select_one yes_no</t>
-  </si>
-  <si>
     <t>reviewed</t>
   </si>
   <si>
     <t>Have you reviewed the Tasks that are due for this client?</t>
   </si>
   <si>
-    <t>select_one status</t>
-  </si>
-  <si>
-    <t>client_status</t>
-  </si>
-  <si>
-    <t>What is the client’s current status?</t>
-  </si>
-  <si>
     <t>recent</t>
   </si>
   <si>
@@ -191,25 +197,16 @@
     <t>No</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>stable</t>
-  </si>
-  <si>
-    <t>Stable</t>
-  </si>
-  <si>
-    <t>unstable</t>
-  </si>
-  <si>
-    <t>Unstable</t>
-  </si>
-  <si>
-    <t>new in care</t>
-  </si>
-  <si>
-    <t>New in care</t>
+    <t>suppressed</t>
+  </si>
+  <si>
+    <t>Suppressed</t>
+  </si>
+  <si>
+    <t>unsuppressed</t>
+  </si>
+  <si>
+    <t>Unsuppressed</t>
   </si>
   <si>
     <t>unknown</t>
@@ -1358,14 +1355,14 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>37</v>
       </c>
+      <c r="B22" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="C22" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1392,16 +1389,16 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="A23" s="10" t="s">
         <v>40</v>
       </c>
+      <c r="B23" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="C23" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1427,13 +1424,13 @@
     </row>
     <row r="24">
       <c r="A24" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1461,15 +1458,15 @@
     </row>
     <row r="25">
       <c r="A25" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="9"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1495,7 +1492,7 @@
     </row>
     <row r="26">
       <c r="A26" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>48</v>
@@ -1529,7 +1526,7 @@
     </row>
     <row r="27">
       <c r="A27" s="11" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>50</v>
@@ -1562,11 +1559,15 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="A28" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1592,7 +1593,9 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1619,6 +1622,34 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
     </row>
+    <row r="30">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1636,7 +1667,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1670,68 +1701,57 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1754,48 +1774,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="14" t="s">
         <v>72</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>73</v>
       </c>
       <c r="H1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="16" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-04-07_17-23</v>
+        <v>2023-07-31_13-56</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>76</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H2" s="2"/>
     </row>

</xml_diff>

<commit_message>
auto:updating the patient identifier card for the routine visit form
</commit_message>
<xml_diff>
--- a/config/forms/app/routine.xlsx
+++ b/config/forms/app/routine.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="114">
   <si>
     <t>type</t>
   </si>
@@ -90,12 +90,21 @@
     <t>patient_id</t>
   </si>
   <si>
+    <t>name1</t>
+  </si>
+  <si>
     <t>date_of_birth</t>
   </si>
   <si>
     <t>sex</t>
   </si>
   <si>
+    <t>tsis</t>
+  </si>
+  <si>
+    <t>genda</t>
+  </si>
+  <si>
     <t>parent</t>
   </si>
   <si>
@@ -123,7 +132,110 @@
     <t>../inputs/contact/name</t>
   </si>
   <si>
+    <t>patient_name1</t>
+  </si>
+  <si>
+    <t>../inputs/contact/name1</t>
+  </si>
+  <si>
+    <t>patient_tsis</t>
+  </si>
+  <si>
+    <t>../inputs/contact/tsis</t>
+  </si>
+  <si>
+    <t>patient_genda</t>
+  </si>
+  <si>
+    <t>../inputs/contact/genda</t>
+  </si>
+  <si>
+    <t>patient_date_of_birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of birth </t>
+  </si>
+  <si>
+    <t>../inputs/contact/date_of_birth</t>
+  </si>
+  <si>
+    <t>date_of_birth_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_date_of_birth != '', instance('contact-summary')/context/patient_date_of_birth, .)</t>
+  </si>
+  <si>
+    <t>aka_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_aka != '', instance('contact-summary')/context/patient_aka, .)</t>
+  </si>
+  <si>
+    <t>fast_name_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/fstname != '', instance('contact-summary')/context/fstname, .)</t>
+  </si>
+  <si>
+    <t>last_name_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/lstname != '', instance('contact-summary')/context/lstname, .)</t>
+  </si>
+  <si>
+    <t>tsis_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_tsis != '', instance('contact-summary')/context/patient_tsis, .)</t>
+  </si>
+  <si>
+    <t>yr_date_of_birth_ctx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int(int(format-date(today(), "%Y") - format-date(${date_of_birth_ctx}, "%Y")) )
+</t>
+  </si>
+  <si>
+    <t>gender_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_genda != '', instance('contact-summary')/context/patient_genda, .)</t>
+  </si>
+  <si>
     <t>routine</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;i style=”background-color: yellow;”&gt;**${fast_name_ctx}  ${last_name_ctx}**&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>nick</t>
+  </si>
+  <si>
+    <t>Nickname: **${aka_ctx}**</t>
+  </si>
+  <si>
+    <t>age_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age: **${yr_date_of_birth_ctx} yr**  </t>
+  </si>
+  <si>
+    <t>gender_n</t>
+  </si>
+  <si>
+    <t>Gender Identity: **${gender_ctx}**</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>TSIS: **${tsis_ctx}**</t>
   </si>
   <si>
     <t>date</t>
@@ -331,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -359,11 +471,23 @@
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -611,7 +735,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="20.25"/>
+    <col customWidth="1" min="2" max="2" width="22.25"/>
     <col customWidth="1" min="3" max="3" width="64.13"/>
+    <col customWidth="1" min="7" max="7" width="49.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -915,13 +1041,13 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="2"/>
@@ -987,17 +1113,19 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1021,17 +1149,19 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1055,19 +1185,17 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1091,19 +1219,17 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>1</v>
+      <c r="A14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1128,10 +1254,14 @@
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1157,13 +1287,19 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
+      <c r="A16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1187,13 +1323,19 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
+      <c r="A17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1218,7 +1360,7 @@
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
@@ -1248,20 +1390,14 @@
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1284,20 +1420,14 @@
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1319,19 +1449,13 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21">
-      <c r="A21" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1355,19 +1479,21 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22">
-      <c r="A22" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>39</v>
+      <c r="A22" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="G22" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1389,19 +1515,21 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23">
-      <c r="A23" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>42</v>
+      <c r="A23" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="G23" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -1423,19 +1551,21 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>45</v>
+      <c r="A24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1457,19 +1587,21 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25">
-      <c r="A25" s="11" t="s">
-        <v>43</v>
+      <c r="A25" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1491,19 +1623,21 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>49</v>
+      <c r="C26" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -1525,19 +1659,21 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27">
-      <c r="A27" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>51</v>
+      <c r="A27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1559,19 +1695,21 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28">
-      <c r="A28" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>53</v>
+      <c r="A28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="G28" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -1594,14 +1732,20 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -1623,13 +1767,21 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="A30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="G30" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -1650,6 +1802,652 @@
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
     </row>
+    <row r="31">
+      <c r="A31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2"/>
+      <c r="Z36" s="2"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+      <c r="Y38" s="2"/>
+      <c r="Z38" s="2"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39" s="2"/>
+      <c r="Z39" s="2"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2"/>
+      <c r="Y41" s="2"/>
+      <c r="Z41" s="2"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+      <c r="Y42" s="2"/>
+      <c r="Z42" s="2"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+      <c r="Y43" s="2"/>
+      <c r="Z43" s="2"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="12"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+      <c r="X44" s="2"/>
+      <c r="Y44" s="2"/>
+      <c r="Z44" s="2"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+      <c r="X45" s="2"/>
+      <c r="Y45" s="2"/>
+      <c r="Z45" s="2"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="2"/>
+      <c r="U46" s="2"/>
+      <c r="V46" s="2"/>
+      <c r="W46" s="2"/>
+      <c r="X46" s="2"/>
+      <c r="Y46" s="2"/>
+      <c r="Z46" s="2"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+      <c r="X47" s="2"/>
+      <c r="Y47" s="2"/>
+      <c r="Z47" s="2"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
+      <c r="U48" s="2"/>
+      <c r="V48" s="2"/>
+      <c r="W48" s="2"/>
+      <c r="X48" s="2"/>
+      <c r="Y48" s="2"/>
+      <c r="Z48" s="2"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
+      <c r="V49" s="2"/>
+      <c r="W49" s="2"/>
+      <c r="X49" s="2"/>
+      <c r="Y49" s="2"/>
+      <c r="Z49" s="2"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1667,7 +2465,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1700,58 +2498,58 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>57</v>
+      <c r="A2" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>59</v>
+      <c r="A3" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>61</v>
+      <c r="A4" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>63</v>
+      <c r="A5" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>65</v>
+      <c r="A6" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1774,48 +2572,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>72</v>
+        <v>103</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="H1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="16" t="str">
+      <c r="A2" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="20" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-07-31_13-56</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17" t="s">
-        <v>76</v>
+        <v>2023-07-31_17-47</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21" t="s">
+        <v>113</v>
       </c>
       <c r="H2" s="2"/>
     </row>

</xml_diff>